<commit_message>
added waiting for connection on reloading
</commit_message>
<xml_diff>
--- a/my number.xlsx
+++ b/my number.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>ahmed 1</t>
-  </si>
-  <si>
     <t>ahmed 2</t>
   </si>
   <si>
@@ -31,6 +28,9 @@
   </si>
   <si>
     <t>ahmed 4</t>
+  </si>
+  <si>
+    <t>أحمد سعيد</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -361,7 +361,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>201120641378</v>
@@ -369,7 +369,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>201120641378</v>
@@ -377,7 +377,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>201120641378</v>
@@ -385,7 +385,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>201120641378</v>

</xml_diff>